<commit_message>
Perubahan pada Scrapping IMDB
</commit_message>
<xml_diff>
--- a/scrapping_imdb/top_picks_data.xlsx
+++ b/scrapping_imdb/top_picks_data.xlsx
@@ -5,17 +5,28 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\scrapping_imdb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9951A71E-3642-4F40-B0E3-F103520B7224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DC2772-3B6B-43E1-8DAA-98FF22A3641C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -917,13 +928,17 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1263,21 +1278,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O45"/>
+  <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="7" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" customWidth="1"/>
     <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" style="4" customWidth="1"/>
+    <col min="15" max="15" width="14" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1308,7 +1330,7 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -1324,7 +1346,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1355,7 +1377,7 @@
       <c r="J2" s="3">
         <v>45424</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="4">
         <v>342247952</v>
       </c>
       <c r="L2">
@@ -1370,8 +1392,9 @@
       <c r="O2" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q2" s="4"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1402,7 +1425,7 @@
       <c r="J3" s="3">
         <v>45375</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="4">
         <v>201199570</v>
       </c>
       <c r="L3">
@@ -1417,8 +1440,10 @@
       <c r="O3" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1449,7 +1474,7 @@
       <c r="J4" s="3">
         <v>45403</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="4">
         <v>41566239</v>
       </c>
       <c r="L4">
@@ -1465,7 +1490,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1496,7 +1521,7 @@
       <c r="J5" s="3">
         <v>45263</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="4">
         <v>115857413</v>
       </c>
       <c r="L5">
@@ -1511,8 +1536,9 @@
       <c r="O5" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q5" s="4"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1543,7 +1569,7 @@
       <c r="J6" s="3">
         <v>44290</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="4">
         <v>470116094</v>
       </c>
       <c r="L6">
@@ -1559,7 +1585,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1590,7 +1616,7 @@
       <c r="J7" s="3">
         <v>45354</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="4">
         <v>711844358</v>
       </c>
       <c r="L7">
@@ -1606,7 +1632,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1637,7 +1663,7 @@
       <c r="J8" s="3">
         <v>45403</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="4">
         <v>25885290</v>
       </c>
       <c r="L8">
@@ -1653,7 +1679,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1684,7 +1710,7 @@
       <c r="J9" s="3">
         <v>43618</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="4">
         <v>387300138</v>
       </c>
       <c r="L9">
@@ -1700,7 +1726,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1723,16 +1749,16 @@
         <v>85000000</v>
       </c>
       <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
+        <v>148753631.93181819</v>
+      </c>
+      <c r="I10" s="4">
+        <v>47359673.340909101</v>
       </c>
       <c r="J10" t="s">
         <v>234</v>
       </c>
-      <c r="K10">
-        <v>0</v>
+      <c r="K10" s="4">
+        <v>425309653.86363637</v>
       </c>
       <c r="L10">
         <v>120</v>
@@ -1747,7 +1773,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1778,7 +1804,7 @@
       <c r="J11" s="3">
         <v>45396</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="4">
         <v>114151795</v>
       </c>
       <c r="L11">
@@ -1794,7 +1820,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1825,7 +1851,7 @@
       <c r="J12" s="3">
         <v>45389</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="4">
         <v>34659562</v>
       </c>
       <c r="L12">
@@ -1841,7 +1867,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1872,7 +1898,7 @@
       <c r="J13" s="3">
         <v>45417</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="4">
         <v>159939817</v>
       </c>
       <c r="L13">
@@ -1888,7 +1914,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1919,7 +1945,7 @@
       <c r="J14" s="3">
         <v>41777</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="4">
         <v>524978362</v>
       </c>
       <c r="L14">
@@ -1935,7 +1961,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1966,7 +1992,7 @@
       <c r="J15" s="3">
         <v>45305</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="4">
         <v>152720535</v>
       </c>
       <c r="L15">
@@ -1982,7 +2008,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -2013,7 +2039,7 @@
       <c r="J16" s="3">
         <v>42806</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="4">
         <v>568652812</v>
       </c>
       <c r="L16">
@@ -2029,7 +2055,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -2052,16 +2078,16 @@
         <v>70000000</v>
       </c>
       <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
+        <v>148753631.93181819</v>
+      </c>
+      <c r="I17" s="4">
+        <v>47359673.340909101</v>
       </c>
       <c r="J17" t="s">
         <v>234</v>
       </c>
-      <c r="K17">
-        <v>0</v>
+      <c r="K17" s="4">
+        <v>425309653.86363637</v>
       </c>
       <c r="L17">
         <v>110</v>
@@ -2076,7 +2102,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -2096,7 +2122,7 @@
         <v>206</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>108388068.18181819</v>
       </c>
       <c r="H18">
         <v>1918403</v>
@@ -2107,7 +2133,7 @@
       <c r="J18" s="3">
         <v>42659</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="4">
         <v>78053145</v>
       </c>
       <c r="L18">
@@ -2122,8 +2148,9 @@
       <c r="O18" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q18" s="4"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -2143,7 +2170,7 @@
         <v>207</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>108388068.18181819</v>
       </c>
       <c r="H19">
         <v>9964512</v>
@@ -2154,7 +2181,7 @@
       <c r="J19" s="3">
         <v>45375</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="4">
         <v>12000477</v>
       </c>
       <c r="L19">
@@ -2170,7 +2197,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -2193,16 +2220,16 @@
         <v>100000000</v>
       </c>
       <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
+        <v>148753631.93181819</v>
+      </c>
+      <c r="I20" s="4">
+        <v>47359673.340909101</v>
       </c>
       <c r="J20" t="s">
         <v>234</v>
       </c>
-      <c r="K20">
-        <v>0</v>
+      <c r="K20" s="4">
+        <v>425309653.86363637</v>
       </c>
       <c r="L20">
         <v>138</v>
@@ -2217,7 +2244,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -2237,22 +2264,22 @@
         <v>209</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>108388068.18181819</v>
       </c>
       <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
+        <v>148753631.93181819</v>
+      </c>
+      <c r="I21" s="4">
+        <v>47359673.340909101</v>
       </c>
       <c r="J21" t="s">
         <v>234</v>
       </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
+      <c r="K21" s="4">
+        <v>425309653.86363637</v>
+      </c>
+      <c r="L21" s="4">
+        <v>128.67768595041323</v>
       </c>
       <c r="M21" t="s">
         <v>12</v>
@@ -2264,7 +2291,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -2295,7 +2322,7 @@
       <c r="J22" s="3">
         <v>42141</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="4">
         <v>380418444</v>
       </c>
       <c r="L22">
@@ -2311,7 +2338,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -2342,7 +2369,7 @@
       <c r="J23" s="3">
         <v>38704</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="4">
         <v>556906378</v>
       </c>
       <c r="L23">
@@ -2358,7 +2385,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -2389,7 +2416,7 @@
       <c r="J24" s="3">
         <v>44493</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="4">
         <v>407573628</v>
       </c>
       <c r="L24">
@@ -2405,7 +2432,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -2436,7 +2463,7 @@
       <c r="J25" s="3">
         <v>44549</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="4">
         <v>1922598219</v>
       </c>
       <c r="L25">
@@ -2452,7 +2479,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -2483,7 +2510,7 @@
       <c r="J26" s="3">
         <v>38116</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="4">
         <v>562711</v>
       </c>
       <c r="L26">
@@ -2499,7 +2526,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -2519,7 +2546,7 @@
         <v>215</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>108388068.18181819</v>
       </c>
       <c r="H27">
         <v>2626127</v>
@@ -2530,7 +2557,7 @@
       <c r="J27" s="3">
         <v>45410</v>
       </c>
-      <c r="K27">
+      <c r="K27" s="4">
         <v>3139717</v>
       </c>
       <c r="L27">
@@ -2546,7 +2573,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -2577,7 +2604,7 @@
       <c r="J28" s="3">
         <v>43205</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="4">
         <v>428128399</v>
       </c>
       <c r="L28">
@@ -2593,7 +2620,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -2624,7 +2651,7 @@
       <c r="J29" s="3">
         <v>42932</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="4">
         <v>490719763</v>
       </c>
       <c r="L29">
@@ -2640,7 +2667,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -2671,7 +2698,7 @@
       <c r="J30" s="3">
         <v>40762</v>
       </c>
-      <c r="K30">
+      <c r="K30" s="4">
         <v>481800873</v>
       </c>
       <c r="L30">
@@ -2687,7 +2714,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -2718,7 +2745,7 @@
       <c r="J31" s="3">
         <v>45130</v>
       </c>
-      <c r="K31">
+      <c r="K31" s="4">
         <v>974954311</v>
       </c>
       <c r="L31">
@@ -2734,7 +2761,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -2765,7 +2792,7 @@
       <c r="J32" s="3">
         <v>41469</v>
       </c>
-      <c r="K32">
+      <c r="K32" s="4">
         <v>411002906</v>
       </c>
       <c r="L32">
@@ -2812,7 +2839,7 @@
       <c r="J33" s="3">
         <v>44780</v>
       </c>
-      <c r="K33">
+      <c r="K33" s="4">
         <v>239268602</v>
       </c>
       <c r="L33">
@@ -2859,7 +2886,7 @@
       <c r="J34" s="3">
         <v>42169</v>
       </c>
-      <c r="K34">
+      <c r="K34" s="4">
         <v>1671537444</v>
       </c>
       <c r="L34">
@@ -2898,16 +2925,16 @@
         <v>100000000</v>
       </c>
       <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35">
-        <v>0</v>
+        <v>148753631.93181819</v>
+      </c>
+      <c r="I35" s="4">
+        <v>47359673.340909101</v>
       </c>
       <c r="J35" t="s">
         <v>234</v>
       </c>
-      <c r="K35">
-        <v>0</v>
+      <c r="K35" s="4">
+        <v>425309653.86363637</v>
       </c>
       <c r="L35">
         <v>180</v>
@@ -2953,7 +2980,7 @@
       <c r="J36" s="3">
         <v>43457</v>
       </c>
-      <c r="K36">
+      <c r="K36" s="4">
         <v>467989645</v>
       </c>
       <c r="L36">
@@ -3000,7 +3027,7 @@
       <c r="J37" s="3">
         <v>41833</v>
       </c>
-      <c r="K37">
+      <c r="K37" s="4">
         <v>710644566</v>
       </c>
       <c r="L37">
@@ -3047,7 +3074,7 @@
       <c r="J38" s="3">
         <v>42155</v>
       </c>
-      <c r="K38">
+      <c r="K38" s="4">
         <v>474609154</v>
       </c>
       <c r="L38">
@@ -3094,7 +3121,7 @@
       <c r="J39" s="3">
         <v>44913</v>
       </c>
-      <c r="K39">
+      <c r="K39" s="4">
         <v>2320250281</v>
       </c>
       <c r="L39">
@@ -3141,7 +3168,7 @@
       <c r="J40" s="3">
         <v>42799</v>
       </c>
-      <c r="K40">
+      <c r="K40" s="4">
         <v>619180476</v>
       </c>
       <c r="L40">
@@ -3188,7 +3215,7 @@
       <c r="J41" s="3">
         <v>45095</v>
       </c>
-      <c r="K41">
+      <c r="K41" s="4">
         <v>271333313</v>
       </c>
       <c r="L41">
@@ -3224,19 +3251,19 @@
         <v>230</v>
       </c>
       <c r="G42">
-        <v>0</v>
+        <v>108388068.18181819</v>
       </c>
       <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="I42">
-        <v>0</v>
+        <v>148753631.93181819</v>
+      </c>
+      <c r="I42" s="4">
+        <v>47359673.340909101</v>
       </c>
       <c r="J42" t="s">
         <v>234</v>
       </c>
-      <c r="K42">
-        <v>0</v>
+      <c r="K42" s="4">
+        <v>425309653.86363637</v>
       </c>
       <c r="L42">
         <v>140</v>
@@ -3282,7 +3309,7 @@
       <c r="J43" s="3">
         <v>43275</v>
       </c>
-      <c r="K43">
+      <c r="K43" s="4">
         <v>1310469037</v>
       </c>
       <c r="L43">
@@ -3329,7 +3356,7 @@
       <c r="J44" s="3">
         <v>35575</v>
       </c>
-      <c r="K44">
+      <c r="K44" s="4">
         <v>618638999</v>
       </c>
       <c r="L44">
@@ -3365,18 +3392,18 @@
         <v>233</v>
       </c>
       <c r="G45">
-        <v>0</v>
+        <v>108388068.18181819</v>
       </c>
       <c r="H45">
-        <v>0</v>
-      </c>
-      <c r="I45">
-        <v>0</v>
+        <v>148753631.93181819</v>
+      </c>
+      <c r="I45" s="4">
+        <v>47359673.340909101</v>
       </c>
       <c r="J45" t="s">
         <v>234</v>
       </c>
-      <c r="K45">
+      <c r="K45" s="4">
         <v>10724345</v>
       </c>
       <c r="L45">

</xml_diff>